<commit_message>
remove stage overlap, rearrange data, save models
</commit_message>
<xml_diff>
--- a/Deliverables/PerformanceRecord.xlsx
+++ b/Deliverables/PerformanceRecord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeby\Proj-SleepAnalysisSRS\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8408C54-9B70-4C66-AEF1-7DECD2B1AC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B66D1E-DFA6-450C-BF55-C4DE6CE4FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="645" windowWidth="12750" windowHeight="9285" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Dataset</t>
   </si>
@@ -54,32 +54,32 @@
     <t>NaN</t>
   </si>
   <si>
-    <t>NREM only</t>
-  </si>
-  <si>
-    <t>REM only</t>
-  </si>
-  <si>
-    <t>P1 (Linear)</t>
-  </si>
-  <si>
-    <t>P1 + P2 (Linear)</t>
-  </si>
-  <si>
-    <t>P(1:4) (Linear)</t>
-  </si>
-  <si>
     <t>P1 (Poly , 2)</t>
   </si>
   <si>
-    <t>Sine Sleep Stage</t>
+    <t>Support Vector Machine - Linear</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P3 </t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +90,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -116,7 +124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -127,8 +135,58 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="thick">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -136,10 +194,103 @@
     <border>
       <left/>
       <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -150,20 +301,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -176,18 +314,129 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thick">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -196,29 +445,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C576D77C-DF2D-4C7F-B9E2-C19C9DB20FAA}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,206 +853,224 @@
     <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" s="38" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="12">
+        <v>77.739999999999995</v>
+      </c>
+      <c r="C3" s="13">
+        <v>41.79</v>
+      </c>
+      <c r="D3" s="12">
+        <v>62.03</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <v>79.91</v>
+      </c>
+      <c r="C4" s="7">
+        <v>59.17</v>
+      </c>
+      <c r="D4" s="6">
+        <v>48.24</v>
+      </c>
+      <c r="E4" s="16">
+        <v>-5.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="24">
+        <v>80.2</v>
+      </c>
+      <c r="C5" s="25">
+        <v>11.68</v>
+      </c>
+      <c r="D5" s="24">
+        <v>78.09</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="38" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>72.86</v>
-      </c>
-      <c r="C2" s="11">
-        <v>43.49</v>
-      </c>
-      <c r="D2" s="2">
-        <v>62.6</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="28">
+        <v>78.31</v>
+      </c>
+      <c r="C7" s="29">
+        <v>42.33</v>
+      </c>
+      <c r="D7" s="28">
+        <v>57.06</v>
+      </c>
+      <c r="E7" s="30">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9">
+        <v>79.91</v>
+      </c>
+      <c r="C8" s="4">
+        <v>56.08</v>
+      </c>
+      <c r="D8" s="2">
+        <v>51.08</v>
+      </c>
+      <c r="E8" s="19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="32">
+        <v>78.709999999999994</v>
+      </c>
+      <c r="C9" s="33">
+        <v>19.91</v>
+      </c>
+      <c r="D9" s="32">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="E9" s="34">
+        <v>13.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>71.72</v>
-      </c>
-      <c r="C3" s="12">
-        <v>40.14</v>
-      </c>
-      <c r="D3" s="3">
-        <v>62.6</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>69.44</v>
-      </c>
-      <c r="C4" s="13">
-        <v>30.75</v>
-      </c>
-      <c r="D4" s="4">
-        <v>62.6</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="C5" s="12">
-        <v>30.75</v>
-      </c>
-      <c r="D5" s="3">
-        <v>62.6</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="B11" s="9">
         <v>49.71</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C11" s="10">
         <v>28.19</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D11" s="9">
         <v>49.03</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E11" s="18">
         <v>-27.87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>78.14</v>
-      </c>
-      <c r="C7" s="12">
-        <v>51.89</v>
-      </c>
-      <c r="D7" s="3">
-        <v>58.41</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4">
-        <v>73.44</v>
-      </c>
-      <c r="C8" s="13">
-        <v>43.94</v>
-      </c>
-      <c r="D8" s="4">
-        <v>63.67</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="9"/>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="10"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="10"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="10"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="9"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="39"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="34"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A10:E10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
NREM REM split and test models
</commit_message>
<xml_diff>
--- a/Deliverables/PerformanceRecord.xlsx
+++ b/Deliverables/PerformanceRecord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeby\Proj-SleepAnalysisSRS\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEF2FDD6-9C6C-4428-B907-C464B8EF90E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FBB0C-6C60-4656-AFAB-EE7F644068C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="2505" windowWidth="16965" windowHeight="11760" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
+    <workbookView xWindow="16680" yWindow="5004" windowWidth="12528" windowHeight="8964" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>Dataset</t>
   </si>
@@ -118,13 +118,19 @@
   </si>
   <si>
     <t>P1:P12</t>
+  </si>
+  <si>
+    <t>P1(REM ONLY)</t>
+  </si>
+  <si>
+    <t>P1(NREM ONLY)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +156,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,18 +196,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -510,13 +524,31 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -525,7 +557,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -547,16 +578,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -578,6 +605,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -587,30 +634,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,68 +967,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C576D77C-DF2D-4C7F-B9E2-C19C9DB20FAA}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="3" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="33" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>77.739999999999995</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>41.79</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>62.03</v>
       </c>
-      <c r="E3" s="50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="E3" s="40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6">
@@ -998,29 +1040,29 @@
       <c r="D4" s="6">
         <v>48.24</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>-5.95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>80.2</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>11.68</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>78.09</v>
       </c>
-      <c r="E5" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="E5" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="6">
@@ -1032,169 +1074,168 @@
       <c r="D6" s="6">
         <v>65.77</v>
       </c>
-      <c r="E6" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="E6" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>84.14</v>
       </c>
-      <c r="C7" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="C7" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
         <v>84.14</v>
       </c>
-      <c r="E7" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="E7" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="6">
         <v>81.98</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="35">
         <v>58.98</v>
       </c>
       <c r="D8" s="6">
         <v>61.58</v>
       </c>
-      <c r="E8" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="E8" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>88.8</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="34">
         <v>46.51</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>88.38</v>
       </c>
-      <c r="E9" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="E9" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="6">
         <v>92.38</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="35">
         <v>45.62</v>
       </c>
       <c r="D10" s="6">
         <v>91.93</v>
       </c>
-      <c r="E10" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="E10" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>79.09</v>
       </c>
-      <c r="C11" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="9">
+      <c r="C11" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
         <v>79.09</v>
       </c>
-      <c r="E11" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="E11" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="6">
         <v>80.709999999999994</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="35">
         <v>26.41</v>
       </c>
       <c r="D12" s="6">
         <v>78.27</v>
       </c>
-      <c r="E12" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="E12" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>89.27</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="34">
         <v>78.08</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>64.86</v>
       </c>
-      <c r="E13" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="E13" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="6">
         <v>85.52</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="35">
         <v>10.85</v>
       </c>
       <c r="D14" s="6">
         <v>85.79</v>
       </c>
-      <c r="E14" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="E14" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>78.03</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>45.67</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>63.61</v>
       </c>
-      <c r="E15" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="E15" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B16" s="36">
         <v>75.150000000000006</v>
       </c>
       <c r="C16" s="5">
@@ -1203,31 +1244,29 @@
       <c r="D16" s="3">
         <v>68.23</v>
       </c>
-      <c r="E16" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="E16" s="39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>75.540000000000006</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>40.32</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>66.989999999999995</v>
       </c>
-      <c r="E17" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="E17" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="6">
@@ -1239,420 +1278,483 @@
       <c r="D18" s="6">
         <v>81.12</v>
       </c>
-      <c r="E18" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="E18" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="8">
         <v>77.81</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="9">
         <v>33.07</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="8">
         <v>73.83</v>
       </c>
-      <c r="E19" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" s="42" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
+      <c r="E19" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3">
+        <v>58.96</v>
+      </c>
+      <c r="C20" s="5">
+        <v>13.8</v>
+      </c>
+      <c r="D20" s="3">
+        <v>61.75</v>
+      </c>
+      <c r="E20" s="18">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="49">
+        <v>84.6</v>
+      </c>
+      <c r="C21" s="50">
+        <v>78.91</v>
+      </c>
+      <c r="D21" s="49">
+        <v>63.32</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="33"/>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B23" s="22">
         <v>78.31</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C23" s="23">
         <v>42.33</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D23" s="22">
         <v>57.06</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E23" s="24">
         <v>3.8</v>
       </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B24" s="8">
         <v>79.91</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C24" s="4">
         <v>56.08</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D24" s="2">
         <v>51.08</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E24" s="17">
         <v>11</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B25" s="3">
         <v>78.709999999999994</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C25" s="5">
         <v>19.91</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D25" s="3">
         <v>77.099999999999994</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E25" s="18">
         <v>13.36</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B26" s="8">
         <v>76.349999999999994</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C26" s="9">
         <v>46.5</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D26" s="8">
         <v>62.79</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E26" s="16">
         <v>0.62</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B27" s="6">
         <v>83.37</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C27" s="7">
         <v>14.19</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D27" s="6">
         <v>83.37</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E27" s="14">
         <v>-7.15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B28" s="8">
         <v>84.27</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C28" s="9">
         <v>54.15</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D28" s="8">
         <v>56.34</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E28" s="16">
         <v>2.8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B29" s="6">
         <v>87.55</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C29" s="7">
         <v>41.46</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D29" s="6">
         <v>88.11</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E29" s="14">
         <v>-2.72</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B30" s="8">
         <v>91.82</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C30" s="9">
         <v>39.42</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D30" s="8">
         <v>91.6</v>
       </c>
-      <c r="E28" s="48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+      <c r="E30" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B31" s="6">
         <v>80.77</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C31" s="7">
         <v>38.79</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D31" s="6">
         <v>78.3</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E31" s="14">
         <v>-6.48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B32" s="8">
         <v>81.02</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C32" s="9">
         <v>33.68</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D32" s="8">
         <v>77.77</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E32" s="16">
         <v>-3.06</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="47" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B33" s="6">
         <v>90.45</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C33" s="7">
         <v>79</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D33" s="6">
         <v>61.08</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E33" s="14">
         <v>2.98</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B34" s="8">
         <v>86.45</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C34" s="9">
         <v>35.29</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D34" s="8">
         <v>85.13</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E34" s="16">
         <v>10.85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B35" s="6">
         <v>78.89</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C35" s="7">
         <v>46.82</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D35" s="6">
         <v>60.3</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E35" s="14">
         <v>6.56</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B36" s="8">
         <v>79.03</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C36" s="9">
         <v>43.29</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D36" s="8">
         <v>66.59</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E36" s="16">
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B37" s="6">
         <v>79.62</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C37" s="7">
         <v>51.33</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D37" s="6">
         <v>65.66</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E37" s="14">
         <v>-0.52</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B38" s="8">
         <v>85.81</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C38" s="4">
         <v>51.17</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D38" s="2">
         <v>80.8</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E38" s="17">
         <v>-2.67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B39" s="3">
         <v>82.4</v>
       </c>
-      <c r="C37" s="31">
+      <c r="C39" s="5">
         <v>50.43</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D39" s="3">
         <v>73.37</v>
       </c>
-      <c r="E37" s="32">
+      <c r="E39" s="18">
         <v>-2.61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="45">
+        <v>60.16</v>
+      </c>
+      <c r="C40" s="46">
+        <v>-0.7</v>
+      </c>
+      <c r="D40" s="45">
+        <v>54.98</v>
+      </c>
+      <c r="E40" s="47">
+        <v>16.78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="53">
+        <v>82.87</v>
+      </c>
+      <c r="C41" s="54">
+        <v>77.53</v>
+      </c>
+      <c r="D41" s="53">
+        <v>62.46</v>
+      </c>
+      <c r="E41" s="55">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="44"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B43" s="8">
         <v>47.8</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C43" s="9">
         <v>-36.18</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D43" s="8">
         <v>55.82</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E43" s="16">
         <v>1.81</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B44" s="3">
         <v>78.31</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C44" s="5">
         <v>42.4</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D44" s="3">
         <v>57.74</v>
       </c>
-      <c r="E40" s="19">
+      <c r="E44" s="18">
         <v>-6.65</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="18"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="19"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="18"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="19"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="19"/>
       <c r="B45" s="2"/>
       <c r="C45" s="4"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="18"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="34"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="32"/>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="20"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="18"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="19"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="17"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="20"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="18"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="19"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="17"/>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="29"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A42:E42"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prep for patient-wise split
</commit_message>
<xml_diff>
--- a/Deliverables/PerformanceRecord.xlsx
+++ b/Deliverables/PerformanceRecord.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeby\Proj-SleepAnalysisSRS\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FBB0C-6C60-4656-AFAB-EE7F644068C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A177123C-B348-4297-B870-02F672D0700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="5004" windowWidth="12528" windowHeight="8964" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
+    <workbookView xWindow="16680" yWindow="5004" windowWidth="12528" windowHeight="8964" activeTab="1" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Pooled Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Patient-Wise Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>Dataset</t>
   </si>
@@ -548,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -653,6 +654,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C576D77C-DF2D-4C7F-B9E2-C19C9DB20FAA}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1760,4 +1766,260 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902475E-F03F-46B2-A4EB-323F27AD8880}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="58"/>
+    </row>
+    <row r="10" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="47"/>
+    </row>
+    <row r="17" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="55"/>
+    </row>
+    <row r="18" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="19"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="19"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="19"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="29"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A18:E18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
prep for feature selection
</commit_message>
<xml_diff>
--- a/Deliverables/PerformanceRecord.xlsx
+++ b/Deliverables/PerformanceRecord.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeby\Proj-SleepAnalysisSRS\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A177123C-B348-4297-B870-02F672D0700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CC8132-BE29-4C5F-93F4-B16931AF79AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="5004" windowWidth="12528" windowHeight="8964" activeTab="1" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
   </bookViews>
   <sheets>
     <sheet name="Pooled Data" sheetId="1" r:id="rId1"/>
     <sheet name="Patient-Wise Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Feature Selection" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="58">
   <si>
     <t>Dataset</t>
   </si>
@@ -124,14 +125,98 @@
     <t>P1(REM ONLY)</t>
   </si>
   <si>
+    <t>NREM</t>
+  </si>
+  <si>
     <t>P1(NREM ONLY)</t>
+  </si>
+  <si>
+    <t>P1:P12(REM ONLY)</t>
+  </si>
+  <si>
+    <t>P1:P12(NREM ONLY)</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>EEG Channels</t>
+  </si>
+  <si>
+    <t>Sleep Stage</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>F4-M1</t>
+  </si>
+  <si>
+    <t>F3-M2</t>
+  </si>
+  <si>
+    <t>C4-M1</t>
+  </si>
+  <si>
+    <t>C3-M2</t>
+  </si>
+  <si>
+    <t>O2-M1</t>
+  </si>
+  <si>
+    <t>01-M2</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>REM</t>
+  </si>
+  <si>
+    <t>WAKE</t>
+  </si>
+  <si>
+    <t>Patient Datasets</t>
+  </si>
+  <si>
+    <t>&lt;Feature Selection Strat&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +254,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +308,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -537,19 +644,352 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -637,7 +1077,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -659,6 +1099,135 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,7 +1545,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1324,7 +1893,7 @@
     </row>
     <row r="21" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="49">
         <v>84.6</v>
@@ -1656,7 +2225,7 @@
     </row>
     <row r="41" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B41" s="53">
         <v>82.87</v>
@@ -1772,13 +2341,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902475E-F03F-46B2-A4EB-323F27AD8880}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
@@ -1860,7 +2429,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="5"/>
@@ -1869,7 +2438,7 @@
     </row>
     <row r="9" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="60" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="50"/>
@@ -1932,7 +2501,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B16" s="45"/>
       <c r="C16" s="46"/>
@@ -1941,7 +2510,7 @@
     </row>
     <row r="17" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="59" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" s="53"/>
       <c r="C17" s="54"/>
@@ -2022,4 +2591,435 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234B6861-C9E6-46F0-8BAF-B7D8E2572558}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" style="66" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="66" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="66" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="66"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="89" customFormat="1" ht="22.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="88"/>
+      <c r="E1" s="65"/>
+    </row>
+    <row r="2" spans="1:5" s="93" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="91"/>
+      <c r="C2" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="92"/>
+      <c r="E2" s="91"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="73"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="61"/>
+      <c r="B5" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="75"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="77"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="61"/>
+      <c r="B6" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="77"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="61"/>
+      <c r="B7" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="77"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="61"/>
+      <c r="B8" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="77"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="63"/>
+      <c r="B9" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="79"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="81"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="73"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="61"/>
+      <c r="B11" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="61"/>
+      <c r="B12" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="75"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="77"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="61"/>
+      <c r="B13" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="75"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="77"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="61"/>
+      <c r="B14" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="75"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="77"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="63"/>
+      <c r="B15" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="79"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="81"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="73"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="61"/>
+      <c r="B17" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="75"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="77"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="61"/>
+      <c r="B18" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="75"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="77"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="61"/>
+      <c r="B19" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="75"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="77"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="61"/>
+      <c r="B20" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="75"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="63"/>
+      <c r="B21" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="79"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="81"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="71"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="73"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="61"/>
+      <c r="B23" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="61"/>
+      <c r="B24" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="75"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="77"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="61"/>
+      <c r="B25" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="75"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="61"/>
+      <c r="B26" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="75"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="77"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="63"/>
+      <c r="B27" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="79"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="81"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="83"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="85"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="61"/>
+      <c r="B29" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="75"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="77"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="61"/>
+      <c r="B30" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="75"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="77"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="61"/>
+      <c r="B31" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="75"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="77"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="61"/>
+      <c r="B32" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="75"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="77"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="61"/>
+      <c r="B33" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="79"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="81"/>
+    </row>
+    <row r="34" spans="1:5" s="93" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="94"/>
+      <c r="C34" s="90" t="str">
+        <f>C2</f>
+        <v>&lt;Feature Selection Strat&gt;</v>
+      </c>
+      <c r="D34" s="92"/>
+      <c r="E34" s="91"/>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="73"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="61"/>
+      <c r="B37" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="75"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="77"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="63"/>
+      <c r="B38" s="78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="79"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="81"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="86"/>
+      <c r="B39" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="101"/>
+      <c r="D39" s="102"/>
+      <c r="E39" s="103"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="87"/>
+      <c r="B40" s="97" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="98"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="100"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A28:A33"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
P2 nrem rem split test
</commit_message>
<xml_diff>
--- a/Deliverables/PerformanceRecord.xlsx
+++ b/Deliverables/PerformanceRecord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeby\Proj-SleepAnalysisSRS\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8809C77B-C6B9-4F16-AD84-6D66F973DA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EED7E31-621C-4F31-9A7D-E8BF893A91B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
+    <workbookView xWindow="15828" yWindow="6384" windowWidth="12528" windowHeight="8964" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
   </bookViews>
   <sheets>
     <sheet name="Pooled Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="60">
   <si>
     <t>Dataset</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>&lt;Feature Selection Strat&gt;</t>
+  </si>
+  <si>
+    <t>P2(REM ONLY)</t>
+  </si>
+  <si>
+    <t>P2(NREM ONLY)</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1233,6 +1239,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1548,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C576D77C-DF2D-4C7F-B9E2-C19C9DB20FAA}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1897,425 +1924,465 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="57" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="107">
         <v>84.6</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="108">
         <v>78.91</v>
       </c>
-      <c r="D21" s="49">
+      <c r="D21" s="107">
         <v>63.32</v>
       </c>
-      <c r="E21" s="51" t="s">
+      <c r="E21" s="109" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="42" t="s">
+    <row r="22" spans="1:5" s="114" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="110" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="111">
+        <v>83.07</v>
+      </c>
+      <c r="C22" s="112">
+        <v>16.29</v>
+      </c>
+      <c r="D22" s="111">
+        <v>81.48</v>
+      </c>
+      <c r="E22" s="113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="49">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="C23" s="50">
+        <v>57.02</v>
+      </c>
+      <c r="D23" s="49">
+        <v>57.93</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="44"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B25" s="22">
         <v>78.31</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C25" s="23">
         <v>42.33</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D25" s="22">
         <v>57.06</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E25" s="24">
         <v>3.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="8">
-        <v>79.91</v>
-      </c>
-      <c r="C24" s="4">
-        <v>56.08</v>
-      </c>
-      <c r="D24" s="2">
-        <v>51.08</v>
-      </c>
-      <c r="E24" s="17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3">
-        <v>78.709999999999994</v>
-      </c>
-      <c r="C25" s="5">
-        <v>19.91</v>
-      </c>
-      <c r="D25" s="3">
-        <v>77.099999999999994</v>
-      </c>
-      <c r="E25" s="18">
-        <v>13.36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="8">
+        <v>79.91</v>
+      </c>
+      <c r="C26" s="4">
+        <v>56.08</v>
+      </c>
+      <c r="D26" s="2">
+        <v>51.08</v>
+      </c>
+      <c r="E26" s="17">
         <v>11</v>
       </c>
-      <c r="B26" s="8">
-        <v>76.349999999999994</v>
-      </c>
-      <c r="C26" s="9">
-        <v>46.5</v>
-      </c>
-      <c r="D26" s="8">
-        <v>62.79</v>
-      </c>
-      <c r="E26" s="16">
-        <v>0.62</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="6">
-        <v>83.37</v>
-      </c>
-      <c r="C27" s="7">
-        <v>14.19</v>
-      </c>
-      <c r="D27" s="6">
-        <v>83.37</v>
-      </c>
-      <c r="E27" s="14">
-        <v>-7.15</v>
+      <c r="A27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="3">
+        <v>78.709999999999994</v>
+      </c>
+      <c r="C27" s="5">
+        <v>19.91</v>
+      </c>
+      <c r="D27" s="3">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="E27" s="18">
+        <v>13.36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B28" s="8">
-        <v>84.27</v>
+        <v>76.349999999999994</v>
       </c>
       <c r="C28" s="9">
-        <v>54.15</v>
+        <v>46.5</v>
       </c>
       <c r="D28" s="8">
-        <v>56.34</v>
+        <v>62.79</v>
       </c>
       <c r="E28" s="16">
-        <v>2.8</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
-        <v>19</v>
+      <c r="A29" s="37" t="s">
+        <v>12</v>
       </c>
       <c r="B29" s="6">
-        <v>87.55</v>
+        <v>83.37</v>
       </c>
       <c r="C29" s="7">
-        <v>41.46</v>
+        <v>14.19</v>
       </c>
       <c r="D29" s="6">
-        <v>88.11</v>
+        <v>83.37</v>
       </c>
       <c r="E29" s="14">
-        <v>-2.72</v>
+        <v>-7.15</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B30" s="8">
-        <v>91.82</v>
+        <v>84.27</v>
       </c>
       <c r="C30" s="9">
-        <v>39.42</v>
+        <v>54.15</v>
       </c>
       <c r="D30" s="8">
-        <v>91.6</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>2</v>
+        <v>56.34</v>
+      </c>
+      <c r="E30" s="16">
+        <v>2.8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="37" t="s">
-        <v>21</v>
+      <c r="A31" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="B31" s="6">
-        <v>80.77</v>
+        <v>87.55</v>
       </c>
       <c r="C31" s="7">
-        <v>38.79</v>
+        <v>41.46</v>
       </c>
       <c r="D31" s="6">
-        <v>78.3</v>
+        <v>88.11</v>
       </c>
       <c r="E31" s="14">
-        <v>-6.48</v>
+        <v>-2.72</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="8">
-        <v>81.02</v>
+        <v>91.82</v>
       </c>
       <c r="C32" s="9">
-        <v>33.68</v>
+        <v>39.42</v>
       </c>
       <c r="D32" s="8">
-        <v>77.77</v>
-      </c>
-      <c r="E32" s="16">
-        <v>-3.06</v>
+        <v>91.6</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="56" t="s">
-        <v>23</v>
+      <c r="A33" s="37" t="s">
+        <v>21</v>
       </c>
       <c r="B33" s="6">
-        <v>90.45</v>
+        <v>80.77</v>
       </c>
       <c r="C33" s="7">
-        <v>79</v>
+        <v>38.79</v>
       </c>
       <c r="D33" s="6">
-        <v>61.08</v>
+        <v>78.3</v>
       </c>
       <c r="E33" s="14">
-        <v>2.98</v>
+        <v>-6.48</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34" s="8">
-        <v>86.45</v>
+        <v>81.02</v>
       </c>
       <c r="C34" s="9">
-        <v>35.29</v>
+        <v>33.68</v>
       </c>
       <c r="D34" s="8">
-        <v>85.13</v>
+        <v>77.77</v>
       </c>
       <c r="E34" s="16">
-        <v>10.85</v>
+        <v>-3.06</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
-        <v>13</v>
+      <c r="A35" s="56" t="s">
+        <v>23</v>
       </c>
       <c r="B35" s="6">
-        <v>78.89</v>
+        <v>90.45</v>
       </c>
       <c r="C35" s="7">
-        <v>46.82</v>
+        <v>79</v>
       </c>
       <c r="D35" s="6">
-        <v>60.3</v>
+        <v>61.08</v>
       </c>
       <c r="E35" s="14">
-        <v>6.56</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B36" s="8">
-        <v>79.03</v>
+        <v>86.45</v>
       </c>
       <c r="C36" s="9">
-        <v>43.29</v>
+        <v>35.29</v>
       </c>
       <c r="D36" s="8">
-        <v>66.59</v>
+        <v>85.13</v>
       </c>
       <c r="E36" s="16">
-        <v>0.05</v>
+        <v>10.85</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B37" s="6">
-        <v>79.62</v>
+        <v>78.89</v>
       </c>
       <c r="C37" s="7">
-        <v>51.33</v>
+        <v>46.82</v>
       </c>
       <c r="D37" s="6">
-        <v>65.66</v>
+        <v>60.3</v>
       </c>
       <c r="E37" s="14">
-        <v>-0.52</v>
+        <v>6.56</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="8">
+        <v>79.03</v>
+      </c>
+      <c r="C38" s="9">
+        <v>43.29</v>
+      </c>
+      <c r="D38" s="8">
+        <v>66.59</v>
+      </c>
+      <c r="E38" s="16">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="6">
+        <v>79.62</v>
+      </c>
+      <c r="C39" s="7">
+        <v>51.33</v>
+      </c>
+      <c r="D39" s="6">
+        <v>65.66</v>
+      </c>
+      <c r="E39" s="14">
+        <v>-0.52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B40" s="8">
         <v>85.81</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C40" s="4">
         <v>51.17</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D40" s="2">
         <v>80.8</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E40" s="17">
         <v>-2.67</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B41" s="3">
         <v>82.4</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C41" s="5">
         <v>50.43</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D41" s="3">
         <v>73.37</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E41" s="18">
         <v>-2.61</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="48" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="45">
+      <c r="B42" s="45">
         <v>60.16</v>
       </c>
-      <c r="C40" s="46">
+      <c r="C42" s="46">
         <v>-0.7</v>
       </c>
-      <c r="D40" s="45">
+      <c r="D42" s="45">
         <v>54.98</v>
       </c>
-      <c r="E40" s="47">
+      <c r="E42" s="47">
         <v>16.78</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="57" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="53">
+      <c r="B43" s="115">
         <v>82.87</v>
       </c>
-      <c r="C41" s="54">
+      <c r="C43" s="116">
         <v>77.53</v>
       </c>
-      <c r="D41" s="53">
+      <c r="D43" s="115">
         <v>62.46</v>
       </c>
-      <c r="E41" s="55">
+      <c r="E43" s="117">
         <v>5.99</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="42" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="45">
+        <v>89.42</v>
+      </c>
+      <c r="C44" s="46">
+        <v>16.29</v>
+      </c>
+      <c r="D44" s="45">
+        <v>80.95</v>
+      </c>
+      <c r="E44" s="118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="106" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="53">
+        <v>78.959999999999994</v>
+      </c>
+      <c r="C45" s="54">
+        <v>63.33</v>
+      </c>
+      <c r="D45" s="53">
+        <v>53.2</v>
+      </c>
+      <c r="E45" s="55">
+        <v>12.46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="44"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="s">
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="44"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B47" s="8">
         <v>47.8</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C47" s="9">
         <v>-36.18</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D47" s="8">
         <v>55.82</v>
       </c>
-      <c r="E43" s="16">
+      <c r="E47" s="16">
         <v>1.81</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B48" s="3">
         <v>78.31</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C48" s="5">
         <v>42.4</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D48" s="3">
         <v>57.74</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E48" s="18">
         <v>-6.65</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="18"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="17"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="18"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="19"/>
@@ -2324,18 +2391,46 @@
       <c r="D49" s="2"/>
       <c r="E49" s="17"/>
     </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="29"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="27"/>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="20"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="18"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="19"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="17"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="20"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="18"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="19"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="17"/>
+    </row>
+    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="29"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A46:E46"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2603,7 +2698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234B6861-C9E6-46F0-8BAF-B7D8E2572558}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
patient split, ahi and write to excel file
</commit_message>
<xml_diff>
--- a/Deliverables/PerformanceRecord.xlsx
+++ b/Deliverables/PerformanceRecord.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeby\Proj-SleepAnalysisSRS\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EED7E31-621C-4F31-9A7D-E8BF893A91B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984ABC60-BA01-47B5-B4DB-505F51C2E1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15828" yWindow="6384" windowWidth="12528" windowHeight="8964" xr2:uid="{8C9CCCCA-55C1-41A4-97D4-EB56A236B105}"/>
+    <workbookView xWindow="7920" yWindow="1725" windowWidth="16965" windowHeight="11760" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pooled Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Patient-Wise Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Feature Selection" sheetId="3" r:id="rId3"/>
+    <sheet name="Patient-Wise Data Copy" sheetId="6" r:id="rId1"/>
+    <sheet name="Pooled Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Patient-Wise Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Feature Selection" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="61">
   <si>
     <t>Dataset</t>
   </si>
@@ -216,6 +217,9 @@
   </si>
   <si>
     <t>P2(NREM ONLY)</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -277,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,31 +296,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,160 +1051,96 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1228,39 +1156,99 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1574,25 +1562,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB253B6-1476-4929-9617-A4FACB0B7BD2}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="91"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="1:5" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="45"/>
+    </row>
+    <row r="18" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="91"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A18:E18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C576D77C-DF2D-4C7F-B9E2-C19C9DB20FAA}">
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="3" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1609,16 +1855,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1631,11 +1877,11 @@
       <c r="D3" s="11">
         <v>62.03</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="104" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1652,7 +1898,7 @@
         <v>-5.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
@@ -1665,11 +1911,11 @@
       <c r="D5" s="8">
         <v>78.09</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
@@ -1682,28 +1928,28 @@
       <c r="D6" s="6">
         <v>65.77</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="116" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="8">
         <v>84.14</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="8">
         <v>84.14</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
@@ -1716,11 +1962,11 @@
       <c r="D8" s="6">
         <v>61.58</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="116" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
@@ -1733,11 +1979,11 @@
       <c r="D9" s="8">
         <v>88.38</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
@@ -1750,28 +1996,28 @@
       <c r="D10" s="6">
         <v>91.93</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="116" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="8">
         <v>79.09</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="8">
         <v>79.09</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>22</v>
       </c>
@@ -1784,12 +2030,12 @@
       <c r="D12" s="6">
         <v>78.27</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="116" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="56" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="8">
@@ -1801,11 +2047,11 @@
       <c r="D13" s="8">
         <v>64.86</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>24</v>
       </c>
@@ -1818,11 +2064,11 @@
       <c r="D14" s="6">
         <v>85.79</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="116" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
@@ -1835,11 +2081,11 @@
       <c r="D15" s="8">
         <v>63.61</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>14</v>
       </c>
@@ -1852,11 +2098,11 @@
       <c r="D16" s="3">
         <v>68.23</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="115" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
@@ -1869,11 +2115,11 @@
       <c r="D17" s="8">
         <v>66.989999999999995</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
@@ -1886,11 +2132,11 @@
       <c r="D18" s="6">
         <v>81.12</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="116" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>27</v>
       </c>
@@ -1903,88 +2149,88 @@
       <c r="D19" s="8">
         <v>73.83</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="48" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="113">
         <v>58.96</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="114">
         <v>13.8</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="113">
         <v>61.75</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="115">
         <v>4.88</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="106" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="107">
+      <c r="B21" s="82">
         <v>84.6</v>
       </c>
-      <c r="C21" s="108">
+      <c r="C21" s="83">
         <v>78.91</v>
       </c>
-      <c r="D21" s="107">
+      <c r="D21" s="82">
         <v>63.32</v>
       </c>
-      <c r="E21" s="109" t="s">
+      <c r="E21" s="106" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="114" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="110" t="s">
+    <row r="22" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="111">
+      <c r="B22" s="109">
         <v>83.07</v>
       </c>
-      <c r="C22" s="112">
+      <c r="C22" s="110">
         <v>16.29</v>
       </c>
-      <c r="D22" s="111">
+      <c r="D22" s="109">
         <v>81.48</v>
       </c>
-      <c r="E22" s="113" t="s">
+      <c r="E22" s="111" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="57" t="s">
+    <row r="23" spans="1:5" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="40">
         <v>79.569999999999993</v>
       </c>
-      <c r="C23" s="50">
+      <c r="C23" s="41">
         <v>57.02</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="40">
         <v>57.93</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="46" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="42" t="s">
+    <row r="24" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="91"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>5</v>
       </c>
@@ -2001,7 +2247,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>6</v>
       </c>
@@ -2018,7 +2264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>7</v>
       </c>
@@ -2035,7 +2281,7 @@
         <v>13.36</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>11</v>
       </c>
@@ -2052,8 +2298,8 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="37" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="117" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="6">
@@ -2069,7 +2315,7 @@
         <v>-7.15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>18</v>
       </c>
@@ -2086,7 +2332,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +2349,7 @@
         <v>-2.72</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>20</v>
       </c>
@@ -2116,12 +2362,12 @@
       <c r="D32" s="8">
         <v>91.6</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="117" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="6">
@@ -2137,7 +2383,7 @@
         <v>-6.48</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>22</v>
       </c>
@@ -2154,8 +2400,8 @@
         <v>-3.06</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="56" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="117" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="6">
@@ -2171,7 +2417,7 @@
         <v>2.98</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>24</v>
       </c>
@@ -2188,7 +2434,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>13</v>
       </c>
@@ -2205,7 +2451,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>14</v>
       </c>
@@ -2222,7 +2468,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>25</v>
       </c>
@@ -2239,7 +2485,7 @@
         <v>-0.52</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>26</v>
       </c>
@@ -2256,7 +2502,7 @@
         <v>-2.67</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>27</v>
       </c>
@@ -2273,84 +2519,84 @@
         <v>-2.61</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="48" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="45">
+      <c r="B42" s="37">
         <v>60.16</v>
       </c>
-      <c r="C42" s="46">
+      <c r="C42" s="38">
         <v>-0.7</v>
       </c>
-      <c r="D42" s="45">
+      <c r="D42" s="37">
         <v>54.98</v>
       </c>
-      <c r="E42" s="47">
+      <c r="E42" s="39">
         <v>16.78</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="106" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="115">
+      <c r="B43" s="85">
         <v>82.87</v>
       </c>
-      <c r="C43" s="116">
+      <c r="C43" s="86">
         <v>77.53</v>
       </c>
-      <c r="D43" s="115">
+      <c r="D43" s="85">
         <v>62.46</v>
       </c>
-      <c r="E43" s="117">
+      <c r="E43" s="87">
         <v>5.99</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="45">
+      <c r="B44" s="37">
         <v>89.42</v>
       </c>
-      <c r="C44" s="46">
+      <c r="C44" s="38">
         <v>16.29</v>
       </c>
-      <c r="D44" s="45">
+      <c r="D44" s="37">
         <v>80.95</v>
       </c>
-      <c r="E44" s="118" t="s">
+      <c r="E44" s="39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="106" t="s">
+    <row r="45" spans="1:5" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="53">
+      <c r="B45" s="43">
         <v>78.959999999999994</v>
       </c>
-      <c r="C45" s="54">
+      <c r="C45" s="44">
         <v>63.33</v>
       </c>
-      <c r="D45" s="53">
+      <c r="D45" s="43">
         <v>53.2</v>
       </c>
-      <c r="E45" s="55">
+      <c r="E45" s="45">
         <v>12.46</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="42" t="s">
+    <row r="46" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="44"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="91"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>3</v>
       </c>
@@ -2367,7 +2613,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>9</v>
       </c>
@@ -2384,42 +2630,42 @@
         <v>-6.65</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="2"/>
       <c r="C49" s="4"/>
       <c r="D49" s="2"/>
       <c r="E49" s="17"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="3"/>
       <c r="C50" s="5"/>
       <c r="D50" s="3"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="2"/>
       <c r="C51" s="4"/>
       <c r="D51" s="2"/>
       <c r="E51" s="17"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="20"/>
       <c r="B52" s="3"/>
       <c r="C52" s="5"/>
       <c r="D52" s="3"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="2"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
       <c r="E53" s="17"/>
     </row>
-    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="29"/>
       <c r="B54" s="25"/>
       <c r="C54" s="26"/>
@@ -2438,26 +2684,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902475E-F03F-46B2-A4EB-323F27AD8880}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="3" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2474,209 +2721,321 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+    <row r="2" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
+        <v>77.255054432348089</v>
+      </c>
+      <c r="C3" s="9">
+        <v>51.390269177523621</v>
+      </c>
+      <c r="D3" s="8">
+        <v>63.646967340590763</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="36">
+        <v>75.464601769911198</v>
+      </c>
+      <c r="C4" s="5">
+        <v>35.917347136114266</v>
+      </c>
+      <c r="D4" s="3">
+        <v>68.230088495575075</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="8">
+        <v>75.808189655172086</v>
+      </c>
+      <c r="C5" s="9">
+        <v>39.590349478347285</v>
+      </c>
+      <c r="D5" s="8">
+        <v>67.474856321838914</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>83.668389814282548</v>
+      </c>
+      <c r="C6" s="7">
+        <v>30.684077217381244</v>
+      </c>
+      <c r="D6" s="6">
+        <v>81.543174420830439</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="8">
+        <v>78.229842446709455</v>
+      </c>
+      <c r="C7" s="9">
+        <v>36.595342692003591</v>
+      </c>
+      <c r="D7" s="8">
+        <v>73.716404077849617</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="60" t="s">
+      <c r="B8" s="3">
+        <v>79.831578947368143</v>
+      </c>
+      <c r="C8" s="88" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3">
+        <v>79.831578947368158</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="58"/>
-    </row>
-    <row r="10" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
+      <c r="B9" s="40">
+        <v>80.336757990867895</v>
+      </c>
+      <c r="C9" s="41">
+        <v>49.744201538047975</v>
+      </c>
+      <c r="D9" s="40">
+        <v>71.48972602739741</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="28" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="44"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="91"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="6">
+        <v>78.227060653187962</v>
+      </c>
+      <c r="C11" s="7">
+        <v>54.68291800562637</v>
+      </c>
+      <c r="D11" s="6">
+        <v>60.031104199066753</v>
+      </c>
+      <c r="E11" s="14">
+        <v>-1.0576287972076925</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="8">
+        <v>78.606194690265013</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45.794925860942158</v>
+      </c>
+      <c r="D12" s="8">
+        <v>65.99557522123844</v>
+      </c>
+      <c r="E12" s="16">
+        <v>-2.1575924583361288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="6">
+        <v>79.418103448275289</v>
+      </c>
+      <c r="C13" s="7">
+        <v>51.801301633854926</v>
+      </c>
+      <c r="D13" s="6">
+        <v>65.499281609194782</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.63298437987879608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="8">
+        <v>86.291403408003546</v>
+      </c>
+      <c r="C14" s="4">
+        <v>47.14425141676184</v>
+      </c>
+      <c r="D14" s="2">
+        <v>81.217690982195023</v>
+      </c>
+      <c r="E14" s="17">
+        <v>-3.1527631431080132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>82.669138090824376</v>
+      </c>
+      <c r="C15" s="5">
+        <v>50.021651122223368</v>
+      </c>
+      <c r="D15" s="3">
+        <v>73.049119555143122</v>
+      </c>
+      <c r="E15" s="18">
+        <v>-0.21417335292714737</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="47"/>
-    </row>
-    <row r="17" spans="1:5" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="59" t="s">
+      <c r="B16" s="37">
+        <v>80.757894736842402</v>
+      </c>
+      <c r="C16" s="38">
+        <v>22.582445150391596</v>
+      </c>
+      <c r="D16" s="37">
+        <v>79.578947368421382</v>
+      </c>
+      <c r="E16" s="39">
+        <v>-4.3882060142790014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="55"/>
-    </row>
-    <row r="18" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="42" t="s">
+      <c r="B17" s="43">
+        <v>83.675799086758431</v>
+      </c>
+      <c r="C17" s="44">
+        <v>55.824538901903111</v>
+      </c>
+      <c r="D17" s="43">
+        <v>70.605022831050903</v>
+      </c>
+      <c r="E17" s="45">
+        <v>1.5208522564238027</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="44"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="91"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="8"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
       <c r="D20" s="3"/>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="E21" s="17"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="3"/>
       <c r="C22" s="5"/>
       <c r="D22" s="3"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="2"/>
       <c r="C23" s="4"/>
       <c r="D23" s="2"/>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="20"/>
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
       <c r="D24" s="3"/>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="2"/>
       <c r="C25" s="4"/>
       <c r="D25" s="2"/>
       <c r="E25" s="17"/>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29"/>
       <c r="B26" s="25"/>
       <c r="C26" s="26"/>
@@ -2694,423 +3053,423 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234B6861-C9E6-46F0-8BAF-B7D8E2572558}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="69" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="69" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="69" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="69"/>
+    <col min="1" max="1" width="13.42578125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="49" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="91" customFormat="1" ht="22.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:5" s="70" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="67" t="s">
+      <c r="B1" s="94"/>
+      <c r="C1" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="68"/>
-    </row>
-    <row r="2" spans="1:5" s="95" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="92" t="s">
+      <c r="D1" s="93"/>
+      <c r="E1" s="94"/>
+    </row>
+    <row r="2" spans="1:5" s="71" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="94" t="s">
+      <c r="B2" s="97"/>
+      <c r="C2" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="93"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="70" t="s">
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="51" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="61"/>
-      <c r="B5" s="76" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="55"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="102"/>
+      <c r="B5" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="79"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="61"/>
-      <c r="B6" s="76" t="s">
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="59"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="102"/>
+      <c r="B6" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="79"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="61"/>
-      <c r="B7" s="76" t="s">
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="59"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="102"/>
+      <c r="B7" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="79"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="61"/>
-      <c r="B8" s="76" t="s">
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="102"/>
+      <c r="B8" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="79"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="66"/>
-      <c r="B9" s="80" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="103"/>
+      <c r="B9" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="65" t="s">
+      <c r="C9" s="61"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="75"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="61"/>
-      <c r="B11" s="76" t="s">
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="55"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="102"/>
+      <c r="B11" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="77"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="79"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="61"/>
-      <c r="B12" s="76" t="s">
+      <c r="C11" s="57"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="102"/>
+      <c r="B12" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="79"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="61"/>
-      <c r="B13" s="76" t="s">
+      <c r="C12" s="57"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="102"/>
+      <c r="B13" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="77"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="61"/>
-      <c r="B14" s="76" t="s">
+      <c r="C13" s="57"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="102"/>
+      <c r="B14" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="77"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="79"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="66"/>
-      <c r="B15" s="80" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="103"/>
+      <c r="B15" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="83"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="65" t="s">
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="75"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="61"/>
-      <c r="B17" s="76" t="s">
+      <c r="C16" s="53"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="102"/>
+      <c r="B17" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="77"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="79"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="61"/>
-      <c r="B18" s="76" t="s">
+      <c r="C17" s="57"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="102"/>
+      <c r="B18" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="77"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="79"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="61"/>
-      <c r="B19" s="76" t="s">
+      <c r="C18" s="57"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="102"/>
+      <c r="B19" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="79"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="61"/>
-      <c r="B20" s="76" t="s">
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="102"/>
+      <c r="B20" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="79"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="66"/>
-      <c r="B21" s="80" t="s">
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="103"/>
+      <c r="B21" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="83"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="65" t="s">
+      <c r="C21" s="61"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="63"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="75"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="61"/>
-      <c r="B23" s="76" t="s">
+      <c r="C22" s="53"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="102"/>
+      <c r="B23" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="79"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="61"/>
-      <c r="B24" s="76" t="s">
+      <c r="C23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="59"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="102"/>
+      <c r="B24" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="79"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="61"/>
-      <c r="B25" s="76" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="102"/>
+      <c r="B25" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="79"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="61"/>
-      <c r="B26" s="76" t="s">
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="102"/>
+      <c r="B26" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="79"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="66"/>
-      <c r="B27" s="80" t="s">
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="103"/>
+      <c r="B27" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="83"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="61" t="s">
+      <c r="C27" s="61"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="85"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="87"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="61"/>
-      <c r="B29" s="76" t="s">
+      <c r="C28" s="65"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="67"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="102"/>
+      <c r="B29" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="77"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="79"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="61"/>
-      <c r="B30" s="76" t="s">
+      <c r="C29" s="57"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="59"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="102"/>
+      <c r="B30" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="77"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="79"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="61"/>
-      <c r="B31" s="76" t="s">
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="102"/>
+      <c r="B31" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="79"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="61"/>
-      <c r="B32" s="76" t="s">
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="59"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="102"/>
+      <c r="B32" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="79"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="61"/>
-      <c r="B33" s="98" t="s">
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="59"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="102"/>
+      <c r="B33" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="99"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="101"/>
-    </row>
-    <row r="34" spans="1:5" s="95" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="102"/>
-      <c r="B34" s="103"/>
-      <c r="C34" s="103"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="104"/>
-    </row>
-    <row r="35" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="92" t="s">
+      <c r="C33" s="75"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="77"/>
+    </row>
+    <row r="34" spans="1:5" s="71" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="78"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="80"/>
+    </row>
+    <row r="35" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="92" t="str">
+      <c r="B35" s="97"/>
+      <c r="C35" s="95" t="str">
         <f>C2</f>
         <v>&lt;Feature Selection Strat&gt;</v>
       </c>
-      <c r="D35" s="94"/>
-      <c r="E35" s="93"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="70" t="s">
+      <c r="D35" s="96"/>
+      <c r="E35" s="97"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="96" t="s">
+      <c r="B36" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="105" t="s">
+      <c r="C36" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="97" t="s">
+      <c r="D36" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="71" t="s">
+      <c r="E36" s="51" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="64" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="73"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="75"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="62"/>
-      <c r="B38" s="76" t="s">
+      <c r="C37" s="53"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="55"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="99"/>
+      <c r="B38" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="77"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="63"/>
-      <c r="B39" s="80" t="s">
+      <c r="C38" s="57"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="59"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="100"/>
+      <c r="B39" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="81"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="83"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="88"/>
-      <c r="B40" s="84" t="s">
+      <c r="C39" s="61"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="63"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="68"/>
+      <c r="B40" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="85"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="87"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="89"/>
-      <c r="B41" s="80" t="s">
+      <c r="C40" s="65"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="67"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="69"/>
+      <c r="B41" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="81"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="83"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>